<commit_message>
Improved loading logic: add null merger, especially improved for ephys data
</commit_message>
<xml_diff>
--- a/cook/thermal_training/status_report.xlsx
+++ b/cook/thermal_training/status_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="99">
   <si>
     <t>Cohort</t>
   </si>
@@ -94,6 +94,9 @@
     <t>20250905</t>
   </si>
   <si>
+    <t>20250906</t>
+  </si>
+  <si>
     <t>20250829_RZJ_3M_Thermal_day3_1_PelSAT50passive</t>
   </si>
   <si>
@@ -199,6 +202,21 @@
     <t>20250905_RZJ_3M_Thermal_day9_5_PelDisLeft50passive</t>
   </si>
   <si>
+    <t>20250906_RZJ_3M_Thermal_day10_1_PelDisLeft50passive</t>
+  </si>
+  <si>
+    <t>20250906_RZJ_3M_Thermal_day10_2_PelDisLeft50passive</t>
+  </si>
+  <si>
+    <t>20250906_RZJ_3M_Thermal_day10_3_PelDisLeft50passive</t>
+  </si>
+  <si>
+    <t>20250906_RZJ_3M_Thermal_day10_4_PelDisLeft50passive</t>
+  </si>
+  <si>
+    <t>20250906_RZJ_3M_Thermal_day10_5_PelDisLeft50passive</t>
+  </si>
+  <si>
     <t>20250830_RZK_15M_Thermal_day1_1_PelSAT50passive</t>
   </si>
   <si>
@@ -272,6 +290,21 @@
   </si>
   <si>
     <t>20250905_RZK_15M_Thermal_day5_5_PelSAT50passive</t>
+  </si>
+  <si>
+    <t>20250906_RZK_15M_Thermal_day6_1_PelSAT50passive</t>
+  </si>
+  <si>
+    <t>20250906_RZK_15M_Thermal_day6_2_PelSAT50passive</t>
+  </si>
+  <si>
+    <t>20250906_RZK_15M_Thermal_day6_3_PelSAT50passive</t>
+  </si>
+  <si>
+    <t>20250906_RZK_15M_Thermal_day6_4_PelSAT50passive</t>
+  </si>
+  <si>
+    <t>20250906_RZK_15M_Thermal_day6_5_PelSAT50passive</t>
   </si>
   <si>
     <t>✅</t>
@@ -672,7 +705,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -740,34 +773,34 @@
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -784,34 +817,34 @@
         <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -828,34 +861,34 @@
         <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -872,34 +905,34 @@
         <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -916,34 +949,34 @@
         <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -960,34 +993,34 @@
         <v>20</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1004,34 +1037,34 @@
         <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1048,34 +1081,34 @@
         <v>20</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1092,34 +1125,34 @@
         <v>20</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1136,34 +1169,34 @@
         <v>20</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1180,34 +1213,34 @@
         <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1224,34 +1257,34 @@
         <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1268,34 +1301,34 @@
         <v>21</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1312,34 +1345,34 @@
         <v>21</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1356,34 +1389,34 @@
         <v>21</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1400,34 +1433,34 @@
         <v>22</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1444,34 +1477,34 @@
         <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1488,34 +1521,34 @@
         <v>22</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1532,34 +1565,34 @@
         <v>22</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1576,34 +1609,34 @@
         <v>22</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1620,34 +1653,34 @@
         <v>23</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1664,34 +1697,34 @@
         <v>23</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1708,34 +1741,34 @@
         <v>23</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1752,34 +1785,34 @@
         <v>23</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1796,34 +1829,34 @@
         <v>23</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -1840,34 +1873,34 @@
         <v>24</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -1884,34 +1917,34 @@
         <v>24</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -1928,34 +1961,34 @@
         <v>24</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -1972,34 +2005,34 @@
         <v>24</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -2016,34 +2049,34 @@
         <v>24</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -2060,34 +2093,34 @@
         <v>25</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -2104,34 +2137,34 @@
         <v>25</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -2148,34 +2181,34 @@
         <v>25</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -2192,34 +2225,34 @@
         <v>25</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -2236,254 +2269,254 @@
         <v>25</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:14">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>16</v>
+      <c r="B37" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>16</v>
+      <c r="B38" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>16</v>
+      <c r="B39" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>16</v>
+      <c r="B40" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>16</v>
+      <c r="B41" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -2497,37 +2530,37 @@
         <v>18</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -2541,37 +2574,37 @@
         <v>18</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2585,37 +2618,37 @@
         <v>18</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -2629,37 +2662,37 @@
         <v>18</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -2673,37 +2706,37 @@
         <v>18</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -2717,37 +2750,37 @@
         <v>18</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N47" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -2761,37 +2794,37 @@
         <v>18</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N48" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:14">
@@ -2805,37 +2838,37 @@
         <v>18</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N49" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:14">
@@ -2849,37 +2882,37 @@
         <v>18</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N50" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:14">
@@ -2893,37 +2926,37 @@
         <v>18</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:14">
@@ -2937,37 +2970,37 @@
         <v>18</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:14">
@@ -2981,37 +3014,37 @@
         <v>18</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:14">
@@ -3025,37 +3058,37 @@
         <v>18</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N54" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:14">
@@ -3069,37 +3102,37 @@
         <v>18</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N55" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:14">
@@ -3113,37 +3146,37 @@
         <v>18</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M56" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N56" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:14">
@@ -3157,37 +3190,37 @@
         <v>18</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L57" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M57" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:14">
@@ -3201,37 +3234,37 @@
         <v>18</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L58" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M58" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -3245,37 +3278,37 @@
         <v>18</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M59" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N59" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:14">
@@ -3289,37 +3322,37 @@
         <v>18</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M60" s="5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="N60" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:14">
@@ -3333,37 +3366,477 @@
         <v>18</v>
       </c>
       <c r="D61" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L61" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M61" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N61" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I61" s="5" t="s">
+      <c r="E62" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="J61" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="K61" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="L61" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="M61" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="N61" s="4" t="s">
-        <v>86</v>
+      <c r="F62" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L62" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M62" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N62" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L63" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M63" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N63" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L64" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M64" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N64" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L65" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M65" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N65" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L66" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M66" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N66" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K67" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L67" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M67" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N67" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K68" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L68" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M68" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N68" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="A69" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L69" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M69" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N69" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="A70" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K70" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L70" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M70" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N70" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J71" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K71" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L71" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M71" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N71" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>